<commit_message>
Created the data provider util for the excel file data that is used in the create api test.
Also added the CreateJobAPIExcelDataDrivenTest and
LoginAPIExcelDataDrivenTest in test-datadriven.xml
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/PhoenixTestData.xlsx
+++ b/src/test/resources/testData/PhoenixTestData.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Srinivas\eclipse-workspace_09_09_2025\PhoenixTestAutomationFramework_RestAssured\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFFB4E80-FE3C-4792-A83E-C2E164A36F3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04A07F8F-30AD-44D1-9FF5-7057933A550E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTestData" sheetId="1" r:id="rId1"/>
+    <sheet name="CreateJobTestData" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="56">
   <si>
     <t>username</t>
   </si>
@@ -40,6 +41,159 @@
   </si>
   <si>
     <t>iamsup</t>
+  </si>
+  <si>
+    <t>mst_service_location_id</t>
+  </si>
+  <si>
+    <t>mst_platform_id</t>
+  </si>
+  <si>
+    <t>mst_warrenty_status_id</t>
+  </si>
+  <si>
+    <t>mst_oem_id</t>
+  </si>
+  <si>
+    <t>customer__first_name</t>
+  </si>
+  <si>
+    <t>customer__last_name</t>
+  </si>
+  <si>
+    <t>customer__mobile_number</t>
+  </si>
+  <si>
+    <t>customer__mobile_number_alt</t>
+  </si>
+  <si>
+    <t>customer__email_id</t>
+  </si>
+  <si>
+    <t>customer__email_id_alt</t>
+  </si>
+  <si>
+    <t>customer_address__flat_number</t>
+  </si>
+  <si>
+    <t>customer_address__apartment_name</t>
+  </si>
+  <si>
+    <t>customer_address__street_name</t>
+  </si>
+  <si>
+    <t>customer_address__landmark</t>
+  </si>
+  <si>
+    <t>customer_address__area</t>
+  </si>
+  <si>
+    <t>customer_address__pincode</t>
+  </si>
+  <si>
+    <t>customer_address__country</t>
+  </si>
+  <si>
+    <t>customer_address__state</t>
+  </si>
+  <si>
+    <t>customer_product__dop</t>
+  </si>
+  <si>
+    <t>customer_product__serial_number</t>
+  </si>
+  <si>
+    <t>customer_product__imei1</t>
+  </si>
+  <si>
+    <t>customer_product__imei2</t>
+  </si>
+  <si>
+    <t>customer_product__popurl</t>
+  </si>
+  <si>
+    <t>customer_product__product_id</t>
+  </si>
+  <si>
+    <t>customer_product__mst_model_id</t>
+  </si>
+  <si>
+    <t>problems__id</t>
+  </si>
+  <si>
+    <t>problems__remark</t>
+  </si>
+  <si>
+    <t>Ariel</t>
+  </si>
+  <si>
+    <t>Collier</t>
+  </si>
+  <si>
+    <t>768-420-0299</t>
+  </si>
+  <si>
+    <t>Tianna.Mante@hotmail.com</t>
+  </si>
+  <si>
+    <t>010</t>
+  </si>
+  <si>
+    <t>blcok2</t>
+  </si>
+  <si>
+    <t>near Podar</t>
+  </si>
+  <si>
+    <t>IJ Kumbhawoods</t>
+  </si>
+  <si>
+    <t>Bangalore south</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Karnataka</t>
+  </si>
+  <si>
+    <t>2025-08-31T18:30:00.000Z</t>
+  </si>
+  <si>
+    <t>battery issue</t>
+  </si>
+  <si>
+    <t>Srinivas</t>
+  </si>
+  <si>
+    <t>Uday</t>
+  </si>
+  <si>
+    <t>Chethan</t>
+  </si>
+  <si>
+    <t>Ramesh</t>
+  </si>
+  <si>
+    <t>Suresh</t>
+  </si>
+  <si>
+    <t>19502790627596</t>
+  </si>
+  <si>
+    <t>19502790627597</t>
+  </si>
+  <si>
+    <t>19502790627598</t>
+  </si>
+  <si>
+    <t>19502790627599</t>
+  </si>
+  <si>
+    <t>19502790627600</t>
+  </si>
+  <si>
+    <t>24502790627601</t>
   </si>
 </sst>
 </file>
@@ -75,8 +229,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -359,8 +514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O25" sqref="O25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -400,4 +555,627 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BBEB007-7792-460E-87A8-2884B3256544}">
+  <dimension ref="A1:AA7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="32.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="25.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="24.44140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="23.21875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="30.109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="22.77734375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="23.5546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="27.21875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="30.109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>21</v>
+      </c>
+      <c r="R1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S1" t="s">
+        <v>23</v>
+      </c>
+      <c r="T1" t="s">
+        <v>24</v>
+      </c>
+      <c r="U1" t="s">
+        <v>25</v>
+      </c>
+      <c r="V1" t="s">
+        <v>26</v>
+      </c>
+      <c r="W1" t="s">
+        <v>27</v>
+      </c>
+      <c r="X1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K2" t="s">
+        <v>36</v>
+      </c>
+      <c r="L2" t="s">
+        <v>37</v>
+      </c>
+      <c r="M2" t="s">
+        <v>38</v>
+      </c>
+      <c r="N2" t="s">
+        <v>39</v>
+      </c>
+      <c r="O2" t="s">
+        <v>40</v>
+      </c>
+      <c r="P2">
+        <v>560083</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>41</v>
+      </c>
+      <c r="R2" t="s">
+        <v>42</v>
+      </c>
+      <c r="S2" t="s">
+        <v>43</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="W2" t="s">
+        <v>43</v>
+      </c>
+      <c r="X2">
+        <v>1</v>
+      </c>
+      <c r="Y2">
+        <v>1</v>
+      </c>
+      <c r="Z2">
+        <v>2</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I3" t="s">
+        <v>35</v>
+      </c>
+      <c r="J3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K3" t="s">
+        <v>36</v>
+      </c>
+      <c r="L3" t="s">
+        <v>37</v>
+      </c>
+      <c r="M3" t="s">
+        <v>38</v>
+      </c>
+      <c r="N3" t="s">
+        <v>39</v>
+      </c>
+      <c r="O3" t="s">
+        <v>40</v>
+      </c>
+      <c r="P3">
+        <v>560083</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>41</v>
+      </c>
+      <c r="R3" t="s">
+        <v>42</v>
+      </c>
+      <c r="S3" t="s">
+        <v>43</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="W3" t="s">
+        <v>43</v>
+      </c>
+      <c r="X3">
+        <v>1</v>
+      </c>
+      <c r="Y3">
+        <v>1</v>
+      </c>
+      <c r="Z3">
+        <v>2</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" t="s">
+        <v>35</v>
+      </c>
+      <c r="K4" t="s">
+        <v>36</v>
+      </c>
+      <c r="L4" t="s">
+        <v>37</v>
+      </c>
+      <c r="M4" t="s">
+        <v>38</v>
+      </c>
+      <c r="N4" t="s">
+        <v>39</v>
+      </c>
+      <c r="O4" t="s">
+        <v>40</v>
+      </c>
+      <c r="P4">
+        <v>560083</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>41</v>
+      </c>
+      <c r="R4" t="s">
+        <v>42</v>
+      </c>
+      <c r="S4" t="s">
+        <v>43</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="W4" t="s">
+        <v>43</v>
+      </c>
+      <c r="X4">
+        <v>1</v>
+      </c>
+      <c r="Y4">
+        <v>1</v>
+      </c>
+      <c r="Z4">
+        <v>2</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5" t="s">
+        <v>34</v>
+      </c>
+      <c r="I5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J5" t="s">
+        <v>35</v>
+      </c>
+      <c r="K5" t="s">
+        <v>36</v>
+      </c>
+      <c r="L5" t="s">
+        <v>37</v>
+      </c>
+      <c r="M5" t="s">
+        <v>38</v>
+      </c>
+      <c r="N5" t="s">
+        <v>39</v>
+      </c>
+      <c r="O5" t="s">
+        <v>40</v>
+      </c>
+      <c r="P5">
+        <v>560083</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>41</v>
+      </c>
+      <c r="R5" t="s">
+        <v>42</v>
+      </c>
+      <c r="S5" t="s">
+        <v>43</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="W5" t="s">
+        <v>43</v>
+      </c>
+      <c r="X5">
+        <v>1</v>
+      </c>
+      <c r="Y5">
+        <v>1</v>
+      </c>
+      <c r="Z5">
+        <v>2</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>48</v>
+      </c>
+      <c r="F6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I6" t="s">
+        <v>35</v>
+      </c>
+      <c r="J6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K6" t="s">
+        <v>36</v>
+      </c>
+      <c r="L6" t="s">
+        <v>37</v>
+      </c>
+      <c r="M6" t="s">
+        <v>38</v>
+      </c>
+      <c r="N6" t="s">
+        <v>39</v>
+      </c>
+      <c r="O6" t="s">
+        <v>40</v>
+      </c>
+      <c r="P6">
+        <v>560083</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>41</v>
+      </c>
+      <c r="R6" t="s">
+        <v>42</v>
+      </c>
+      <c r="S6" t="s">
+        <v>43</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="W6" t="s">
+        <v>43</v>
+      </c>
+      <c r="X6">
+        <v>1</v>
+      </c>
+      <c r="Y6">
+        <v>1</v>
+      </c>
+      <c r="Z6">
+        <v>2</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I7" t="s">
+        <v>35</v>
+      </c>
+      <c r="J7" t="s">
+        <v>35</v>
+      </c>
+      <c r="K7" t="s">
+        <v>36</v>
+      </c>
+      <c r="L7" t="s">
+        <v>37</v>
+      </c>
+      <c r="M7" t="s">
+        <v>38</v>
+      </c>
+      <c r="N7" t="s">
+        <v>39</v>
+      </c>
+      <c r="O7" t="s">
+        <v>40</v>
+      </c>
+      <c r="P7">
+        <v>560083</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>41</v>
+      </c>
+      <c r="R7" t="s">
+        <v>42</v>
+      </c>
+      <c r="S7" t="s">
+        <v>43</v>
+      </c>
+      <c r="T7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="U7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="W7" t="s">
+        <v>43</v>
+      </c>
+      <c r="X7">
+        <v>1</v>
+      </c>
+      <c r="Y7">
+        <v>1</v>
+      </c>
+      <c r="Z7">
+        <v>2</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>